<commit_message>
Business questions and actionable insights
The file contains business questions, the columns and tables for the queries, the answers, and actionable insights.
</commit_message>
<xml_diff>
--- a/NFT Business Questions.xlsx
+++ b/NFT Business Questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\old_d\ziva pc\Jundatyst\NFT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49A13F0-B998-4377-81AD-3EA0772C0B49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F2F949-E26E-42A5-BF0D-8C9A28CFD458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -228,10 +228,6 @@
 </t>
   </si>
   <si>
-    <t>Can offer discounts, special deals, promotions etc. to the "heavy" (VIP) minters.
-Should also consider giving an incentive for minting more than 20 NFTs</t>
-  </si>
-  <si>
     <t>Which users (addresses) sold the most amount of NFTs (either minters or buyers)?</t>
   </si>
   <si>
@@ -265,11 +261,6 @@
 2. mints_day_of_week
 3. TRANSFERS_TIME_OF_DAY
 4. MINTS_TIME_OF_DAY</t>
-  </si>
-  <si>
-    <t>* Most mints occured on Friday.
-* Most transfer transactions occured on Sunday.
-* Both mints and transfers strongest hour of the day is 22:00.</t>
   </si>
   <si>
     <t>Can come up with special deals on other days of the week/ times of day to incentivize more transactions</t>
@@ -378,6 +369,15 @@
   <si>
     <t>The median holding time is around 10 days, which seem to contradict our findings regarding the number of times unique NFTs are sold (once, in the majority of cases, and an average of 1.65 times).
 A possible explanation to this contradiction is that we found a huge spike in the volume of transfer transactions towards the end of our dataset, which might be skewing the median holding time downwards</t>
+  </si>
+  <si>
+    <t>* Most mints occured on Friday.
+* Most transfer transactions occured on Sunday.
+* Both mints' and transfers' strongest hour of the day is 22:00.</t>
+  </si>
+  <si>
+    <t>Can offer discounts, special deals, promotions etc. to the high volume (VIP) minters.
+Should also consider giving an incentive for minting more than 20 NFTs</t>
   </si>
 </sst>
 </file>
@@ -561,10 +561,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -583,6 +579,10 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -862,8 +862,8 @@
   <dimension ref="A1:AC995"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -882,31 +882,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="24" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -926,7 +926,7 @@
       </c>
     </row>
     <row r="2" spans="1:29" ht="170.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="25" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -949,7 +949,7 @@
         <v>20</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>21</v>
@@ -977,7 +977,7 @@
       <c r="AC2" s="9"/>
     </row>
     <row r="3" spans="1:29" ht="159" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="25" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -1000,7 +1000,7 @@
         <v>24</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J3" s="8" t="s">
         <v>21</v>
@@ -1028,7 +1028,7 @@
       <c r="AC3" s="9"/>
     </row>
     <row r="4" spans="1:29" ht="174.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="25" t="s">
         <v>25</v>
       </c>
       <c r="B4" s="5"/>
@@ -1051,7 +1051,7 @@
         <v>29</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J4" s="8" t="s">
         <v>21</v>
@@ -1079,7 +1079,7 @@
       <c r="AC4" s="9"/>
     </row>
     <row r="5" spans="1:29" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="25" t="s">
         <v>30</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -1102,7 +1102,7 @@
         <v>35</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
@@ -1126,7 +1126,7 @@
       <c r="AC5" s="9"/>
     </row>
     <row r="6" spans="1:29" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="25" t="s">
         <v>36</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -1149,7 +1149,7 @@
         <v>37</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J6" s="8"/>
       <c r="K6" s="8" t="s">
@@ -1175,7 +1175,7 @@
       <c r="AC6" s="9"/>
     </row>
     <row r="7" spans="1:29" ht="126" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="25" t="s">
         <v>39</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -1200,7 +1200,7 @@
         <v>45</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
@@ -1224,7 +1224,7 @@
       <c r="AC7" s="9"/>
     </row>
     <row r="8" spans="1:29" ht="285.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="25" t="s">
         <v>46</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -1245,14 +1245,14 @@
         <v>49</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
       <c r="N8" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="O8" s="9"/>
       <c r="P8" s="9"/>
@@ -1271,7 +1271,7 @@
       <c r="AC8" s="9"/>
     </row>
     <row r="9" spans="1:29" ht="180.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="25" t="s">
         <v>50</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -1291,10 +1291,10 @@
         <v>52</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
@@ -1318,7 +1318,7 @@
       <c r="AC9" s="9"/>
     </row>
     <row r="10" spans="1:29" ht="175.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="25" t="s">
         <v>53</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -1338,10 +1338,10 @@
         <v>52</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
@@ -1365,8 +1365,8 @@
       <c r="AC10" s="9"/>
     </row>
     <row r="11" spans="1:29" ht="145.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="27" t="s">
-        <v>90</v>
+      <c r="A11" s="25" t="s">
+        <v>88</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>54</v>
@@ -1388,10 +1388,10 @@
         <v>57</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>58</v>
+        <v>94</v>
       </c>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
@@ -1415,7 +1415,7 @@
     </row>
     <row r="12" spans="1:29" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>54</v>
@@ -1431,27 +1431,27 @@
         <v>43</v>
       </c>
       <c r="G12" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H12" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H12" s="4" t="s">
-        <v>61</v>
-      </c>
       <c r="I12" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="J12" s="7" t="s">
         <v>86</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>88</v>
       </c>
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
       <c r="M12" s="8"/>
       <c r="N12" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:29" ht="129.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>54</v>
@@ -1467,57 +1467,57 @@
         <v>43</v>
       </c>
       <c r="G13" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H13" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="I13" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="J13" s="7" t="s">
         <v>63</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="J13" s="7" t="s">
-        <v>64</v>
       </c>
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
       <c r="M13" s="8"/>
       <c r="N13" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:29" ht="191.25" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="12"/>
       <c r="E14" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>33</v>
       </c>
       <c r="G14" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="J14" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="K14" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="J14" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="K14" s="7" t="s">
-        <v>71</v>
       </c>
       <c r="L14" s="8"/>
       <c r="M14" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="N14" s="8"/>
     </row>
@@ -1534,21 +1534,21 @@
       <c r="I16" s="13"/>
     </row>
     <row r="17" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
+      <c r="A17" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14"/>
     </row>
     <row r="18" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
@@ -1561,12 +1561,12 @@
     </row>
     <row r="19" spans="1:9" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C19" s="17"/>
       <c r="D19" s="19"/>
       <c r="E19" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F19" s="18"/>
       <c r="G19" s="18"/>
@@ -1575,13 +1575,13 @@
     </row>
     <row r="20" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B20" s="17"/>
       <c r="C20" s="16"/>
       <c r="D20" s="16"/>
       <c r="E20" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F20" s="18"/>
       <c r="G20" s="18"/>
@@ -7466,72 +7466,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="21"/>
+    </row>
+    <row r="3" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="21"/>
+    </row>
+    <row r="4" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="21" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="21" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="23"/>
-    </row>
-    <row r="3" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="23"/>
-    </row>
-    <row r="4" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="23" t="s">
+    <row r="6" spans="1:1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="21" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="23" t="s">
+    <row r="7" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="20" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="23" t="s">
+    <row r="8" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A8" s="20" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="22" t="s">
+    <row r="9" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="22"/>
+    </row>
+    <row r="10" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="22"/>
+    </row>
+    <row r="11" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="22"/>
+    </row>
+    <row r="12" spans="1:1" ht="108" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="21" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="22" t="s">
+    <row r="13" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="22"/>
+    </row>
+    <row r="14" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="22"/>
+    </row>
+    <row r="15" spans="1:1" ht="344.25" x14ac:dyDescent="0.2">
+      <c r="A15" s="21" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="24"/>
-    </row>
-    <row r="10" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="24"/>
-    </row>
-    <row r="11" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="24"/>
-    </row>
-    <row r="12" spans="1:1" ht="108" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="23" t="s">
+    <row r="16" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="22"/>
+    </row>
+    <row r="17" spans="1:1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A17" s="21" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="24"/>
-    </row>
-    <row r="14" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="24"/>
-    </row>
-    <row r="15" spans="1:1" ht="344.25" x14ac:dyDescent="0.2">
-      <c r="A15" s="23" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="24"/>
-    </row>
-    <row r="17" spans="1:1" ht="102" x14ac:dyDescent="0.2">
-      <c r="A17" s="23" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>